<commit_message>
LBCB 3 calibration fixes.
</commit_message>
<xml_diff>
--- a/Config/Calibrations/LBCB3DisplacementCals.xlsx
+++ b/Config/Calibrations/LBCB3DisplacementCals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="19005" windowHeight="15990"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="19005" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Displacement Cals" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
   <si>
     <t>X1</t>
   </si>
@@ -92,7 +92,7 @@
     <t>Mid-Point</t>
   </si>
   <si>
-    <t>Full Retraction After Y1 Calibration</t>
+    <t>Expected</t>
   </si>
 </sst>
 </file>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,24 +1928,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
@@ -1954,18 +1954,14 @@
         <v>18</v>
       </c>
       <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1979,138 +1975,199 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
       <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="M2">
+        <v>5.9370000000000003</v>
+      </c>
+      <c r="N2">
+        <f>M2-M3</f>
+        <v>-1.2999999999999901E-2</v>
+      </c>
+      <c r="O2">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>-70.11</v>
+        <v>-99.35</v>
       </c>
       <c r="C3">
-        <v>7.3630000000000004</v>
+        <v>10.3202</v>
       </c>
       <c r="D3">
-        <v>72.09</v>
+        <v>0.9</v>
       </c>
       <c r="E3">
-        <v>-7.5579999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-9.2989699999999995E-2</v>
+      </c>
+      <c r="M3">
+        <v>5.95</v>
+      </c>
+      <c r="O3">
+        <v>48.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>-72.010000000000005</v>
+        <v>-98.39</v>
       </c>
       <c r="C4" s="3">
-        <v>7.4619999999999997</v>
+        <v>10.237</v>
       </c>
       <c r="D4">
-        <v>71.08</v>
+        <v>0.45</v>
       </c>
       <c r="E4">
-        <v>-7.3860000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-5.0712E-2</v>
+      </c>
+      <c r="O4">
+        <v>48.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>-71.03</v>
+        <v>-99</v>
       </c>
       <c r="C5">
-        <v>7.3159999999999998</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="D5">
-        <v>72.72</v>
+        <v>1.31</v>
       </c>
       <c r="E5" s="3">
-        <v>-7.4530000000000003</v>
+        <v>-0.1043</v>
       </c>
       <c r="F5">
-        <v>72.72</v>
-      </c>
-      <c r="G5" s="3">
-        <v>-7.4530000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <f>1.03</f>
+        <v>1.03</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>4.9615200000000002</v>
+      </c>
+      <c r="I5">
+        <v>6.03</v>
+      </c>
+      <c r="M5">
+        <v>5.97</v>
+      </c>
+      <c r="O5">
+        <v>-48.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="D6">
-        <v>73.22</v>
+        <v>0.09</v>
       </c>
       <c r="E6">
-        <v>-7.5259999999999998</v>
+        <v>-1.63535E-2</v>
       </c>
       <c r="F6">
-        <v>73.22</v>
+        <v>1.03</v>
       </c>
       <c r="G6">
-        <v>-7.5259999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-48.58</v>
+      </c>
+      <c r="H6">
+        <v>4.8705800000000004</v>
+      </c>
+      <c r="I6">
+        <v>6.03</v>
+      </c>
+      <c r="J6">
+        <v>6.03</v>
+      </c>
+      <c r="M6">
+        <v>6.02</v>
+      </c>
+      <c r="O6">
+        <v>-49.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2">
-        <v>70.64</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E7" s="3">
-        <v>-7.2960000000000003</v>
-      </c>
-      <c r="F7" s="2">
-        <v>70.64</v>
-      </c>
-      <c r="G7" s="3">
-        <v>-7.2960000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-0.10027899999999999</v>
+      </c>
+      <c r="F7">
+        <v>1.03</v>
+      </c>
+      <c r="G7">
+        <v>-48.4</v>
+      </c>
+      <c r="H7">
+        <v>5.0345399999999998</v>
+      </c>
+      <c r="I7">
+        <v>6.03</v>
+      </c>
+      <c r="O7">
+        <v>-49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="D8">
-        <v>76.489999999999995</v>
+        <v>0.26</v>
       </c>
       <c r="E8">
-        <v>-7.891</v>
+        <v>-2.17311E-2</v>
       </c>
       <c r="F8">
-        <v>76.489999999999995</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>-7.891</v>
+        <v>-49</v>
+      </c>
+      <c r="H8">
+        <v>5.0624599999999997</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>